<commit_message>
fixing a couple typos
</commit_message>
<xml_diff>
--- a/form-files/IMNCI/IMNCI.xlsx
+++ b/form-files/IMNCI/IMNCI.xlsx
@@ -3132,10 +3132,10 @@
     <t>schema.type</t>
   </si>
   <si>
-    <t>shema.properties.pulse.type</t>
-  </si>
-  <si>
-    <t>shema.properties.ox.type</t>
+    <t>schema.properties.pulse.type</t>
+  </si>
+  <si>
+    <t>schema.properties.ox.type</t>
   </si>
   <si>
     <t>object</t>

</xml_diff>

<commit_message>
Renaming settings to use underscores.
</commit_message>
<xml_diff>
--- a/form-files/IMNCI/IMNCI.xlsx
+++ b/form-files/IMNCI/IMNCI.xlsx
@@ -4258,22 +4258,22 @@
     <t>value.hindi</t>
   </si>
   <si>
-    <t>formId</t>
+    <t>form_id</t>
   </si>
   <si>
     <t>imnci</t>
   </si>
   <si>
-    <t>formVersion</t>
-  </si>
-  <si>
-    <t>formTitle</t>
+    <t>form_version</t>
+  </si>
+  <si>
+    <t>form_title</t>
   </si>
   <si>
     <t>IMNCI</t>
   </si>
   <si>
-    <t>tableId</t>
+    <t>table_id</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Regen with javascript XLSXConverter (after fixing explicit model bug).
</commit_message>
<xml_diff>
--- a/form-files/IMNCI/IMNCI.xlsx
+++ b/form-files/IMNCI/IMNCI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="228" yWindow="564" windowWidth="26556" windowHeight="12372"/>
+    <workbookView xWindow="84" yWindow="2640" windowWidth="26556" windowHeight="8532" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="survey.2_gt2mo" sheetId="1" r:id="rId1"/>
@@ -4964,7 +4964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A131" workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -15960,7 +15960,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16995,7 +16995,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17027,7 +17029,7 @@
         <v>1355</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>20130408</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">

</xml_diff>